<commit_message>
TO92 test socket, Ingun, Ampenol, M.2 SSD
</commit_message>
<xml_diff>
--- a/Branded/Ingun/Probes.xlsx
+++ b/Branded/Ingun/Probes.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoeren\Desktop\ingun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoeren\Desktop\Repos\Semi-ATE\3D-Models\Branded\Ingun\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F04851-73E3-4207-A2CF-249AD3B7D6EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21945" windowHeight="9135"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Hören Tom</author>
   </authors>
   <commentList>
-    <comment ref="J15" authorId="0" shapeId="0">
+    <comment ref="J15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -53,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J16" authorId="0" shapeId="0">
+    <comment ref="J16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -114,9 +115,6 @@
     <t>14 crown, 4-point, self-cleaning</t>
   </si>
   <si>
-    <t>E-050 214 050 A 2000</t>
-  </si>
-  <si>
     <t>E-050</t>
   </si>
   <si>
@@ -199,12 +197,15 @@
   </si>
   <si>
     <t>GKS-050-314-050-A-1500</t>
+  </si>
+  <si>
+    <t>E-050-214-050-A-2000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -555,11 +556,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B9:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +578,7 @@
   <sheetData>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
@@ -592,10 +593,10 @@
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
         <v>2</v>
@@ -621,10 +622,10 @@
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
@@ -633,16 +634,16 @@
         <v>9</v>
       </c>
       <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="I13" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="J13" t="s">
         <v>8</v>
@@ -650,28 +651,28 @@
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
         <v>23</v>
       </c>
-      <c r="C14" t="s">
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" t="s">
         <v>16</v>
       </c>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="H14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="J14" t="s">
         <v>8</v>
@@ -679,45 +680,45 @@
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" t="s">
         <v>34</v>
       </c>
-      <c r="F15" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>35</v>
       </c>
-      <c r="I15" t="s">
-        <v>36</v>
-      </c>
       <c r="J15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -726,10 +727,10 @@
     <mergeCell ref="H11:I11"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G13" r:id="rId1"/>
-    <hyperlink ref="I13" r:id="rId2"/>
-    <hyperlink ref="G14" r:id="rId3"/>
-    <hyperlink ref="I14" r:id="rId4"/>
+    <hyperlink ref="G13" r:id="rId1" display="E-050 214 050 A 2000" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="I13" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G14" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="I14" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>